<commit_message>
Fix autocorrect in ar translation xls
</commit_message>
<xml_diff>
--- a/docassemble/ALKilnTests/data/sources/ar.xlsx
+++ b/docassemble/ALKilnTests/data/sources/ar.xlsx
@@ -49,7 +49,7 @@
     <t>en</t>
   </si>
   <si>
-    <t>are</t>
+    <t>ar</t>
   </si>
   <si>
     <t>English page</t>
@@ -151,7 +151,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="right" vertical="bottom" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>

</xml_diff>